<commit_message>
SIgnificant changes and works fine
</commit_message>
<xml_diff>
--- a/resources/testdata.xlsx
+++ b/resources/testdata.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\M1089261\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\M1089261\Downloads\tide-final\tide\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA53876D-C17A-44EA-B243-7348E16983D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1CF38F6-87FA-4EB4-8D3A-96C96F4BFB44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1400" yWindow="1400" windowWidth="14400" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tide test data" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="42">
   <si>
     <t>Data</t>
   </si>
@@ -149,6 +149,9 @@
   </si>
   <si>
     <t>initial message to be sent to chat agent in the chat window</t>
+  </si>
+  <si>
+    <t>hello@tide.com</t>
   </si>
 </sst>
 </file>
@@ -492,7 +495,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:D13"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -567,7 +570,7 @@
         <v>8</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>9</v>
+        <v>41</v>
       </c>
       <c r="D5" t="s">
         <v>13</v>
@@ -688,7 +691,7 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C3" r:id="rId1" xr:uid="{3EACED1E-AD63-4BB7-BA48-46811295F153}"/>
-    <hyperlink ref="C5" r:id="rId2" xr:uid="{C41F2836-D9AC-4137-9B9F-ABC5AC4627F3}"/>
+    <hyperlink ref="C5" r:id="rId2" display="hellothere@tide.com" xr:uid="{C41F2836-D9AC-4137-9B9F-ABC5AC4627F3}"/>
     <hyperlink ref="C6" r:id="rId3" xr:uid="{BFEC5D93-AAE4-48D4-ACFB-EB9E65F8B973}"/>
     <hyperlink ref="C4" r:id="rId4" xr:uid="{44DB1BDD-8E58-45B4-A19C-143FA6C336CA}"/>
     <hyperlink ref="C12" r:id="rId5" xr:uid="{E9BEB97F-078D-4253-800A-9ECAA745EFA4}"/>

</xml_diff>